<commit_message>
updated data with Tagi-data, added new columns for forecast
</commit_message>
<xml_diff>
--- a/data_vaccines.xlsx
+++ b/data_vaccines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{B60E0DC6-7A11-471E-8F97-95DB1CC7DC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{620BFA2B-9438-4388-B526-3B23BB7DFE71}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DC0145-15ED-4B77-91A7-0142340774B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="3792" windowWidth="30612" windowHeight="9432" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccine approval" sheetId="3" r:id="rId1"/>
@@ -36,9 +36,27 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}</author>
+    <author>tc={DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}</author>
+    <author>tc={21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}</author>
   </authors>
   <commentList>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
+      </text>
+    </comment>
+    <comment ref="I18" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -51,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="32">
   <si>
     <t>country</t>
   </si>
@@ -116,9 +134,6 @@
     <t>https://www.srf.ch/news/schweiz/mehr-impfstoff-in-sicht-126-000-neue-impfdosen-bag-wehrt-sich-gegen-kritik</t>
   </si>
   <si>
-    <t>https://www.cash.ch/news/politik/coronavirus-update-corona-bag-meldet-4020-neue-coronavirus-infektionen-schweiz-hat-233000-1688758</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -138,19 +153,30 @@
   </si>
   <si>
     <t>https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert</t>
+  </si>
+  <si>
+    <t>shipping_volume_forecast</t>
+  </si>
+  <si>
+    <t>BAG pdf</t>
+  </si>
+  <si>
+    <t>https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/</t>
+  </si>
+  <si>
+    <t>shipping_volume_forecast_cummulated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -175,6 +201,12 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -206,7 +238,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -219,9 +251,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -545,7 +578,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I15" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+  <threadedComment ref="I17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
+  </threadedComment>
+  <threadedComment ref="I18" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+    <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
+  </threadedComment>
+  <threadedComment ref="I19" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
 </ThreadedComments>
@@ -553,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B207B-0EB6-4EF4-88FB-421592296A82}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K5:M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -564,11 +603,14 @@
     <col min="3" max="3" width="79.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="21.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="4"/>
+    <col min="13" max="15" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -602,17 +644,23 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -647,18 +695,20 @@
       <c r="K2" s="1">
         <v>44184</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
         <f>SUM(L$2:L2)</f>
         <v>0</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -693,18 +743,20 @@
       <c r="K3" s="1">
         <v>44185</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>107000</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <f>SUM(L$2:L3)</f>
         <v>107000</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -739,26 +791,28 @@
       <c r="K4" s="1">
         <v>44200</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>126000</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <f>SUM(L$2:L4)</f>
         <v>233000</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>44201</v>
+        <v>44228</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -773,7 +827,7 @@
         <v>3000000</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H9" si="0">G5/I5</f>
+        <f t="shared" ref="H5" si="0">G5/I5</f>
         <v>1500000</v>
       </c>
       <c r="I5" s="4">
@@ -783,28 +837,27 @@
         <v>18</v>
       </c>
       <c r="K5" s="1">
-        <v>44227</v>
-      </c>
-      <c r="L5">
-        <v>500000</v>
-      </c>
-      <c r="M5">
-        <f>SUM(L$2:L5)</f>
-        <v>733000</v>
-      </c>
-      <c r="N5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44220</v>
+      </c>
+      <c r="L5" s="4">
+        <f>M5-M4</f>
+        <v>38400</v>
+      </c>
+      <c r="M5" s="4">
+        <v>271400</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1">
-        <v>44201</v>
+        <v>44228</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -819,7 +872,7 @@
         <v>3000000</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H6" si="1">G6/I6</f>
         <v>1500000</v>
       </c>
       <c r="I6" s="4">
@@ -829,25 +882,27 @@
         <v>18</v>
       </c>
       <c r="K6" s="1">
-        <v>44255</v>
-      </c>
-      <c r="L6">
-        <v>500000</v>
-      </c>
-      <c r="M6">
-        <f>SUM(L$2:L6)</f>
-        <v>1233000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44223</v>
+      </c>
+      <c r="L6" s="4">
+        <f>M6-M5</f>
+        <v>60460</v>
+      </c>
+      <c r="M6" s="4">
+        <v>331860</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>44201</v>
+        <v>44228</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -862,7 +917,7 @@
         <v>3000000</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="0"/>
+        <f>G7/I7</f>
         <v>1500000</v>
       </c>
       <c r="I7" s="4">
@@ -872,25 +927,29 @@
         <v>18</v>
       </c>
       <c r="K7" s="1">
-        <v>44286</v>
-      </c>
-      <c r="L7">
-        <v>500000</v>
-      </c>
-      <c r="M7">
-        <f>SUM(L$2:L7)</f>
-        <v>1733000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44228</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4">
+        <v>22217</v>
+      </c>
+      <c r="O7" s="4">
+        <f>SUM(N$7:N7)+M$6</f>
+        <v>354077</v>
+      </c>
+      <c r="P7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1">
-        <v>44201</v>
+        <v>44228</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -905,7 +964,7 @@
         <v>3000000</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" ref="H8" si="1">G8/I8</f>
+        <f>G8/I8</f>
         <v>1500000</v>
       </c>
       <c r="I8" s="4">
@@ -915,36 +974,42 @@
         <v>18</v>
       </c>
       <c r="K8" s="1">
-        <v>44316</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f>SUM(L$2:L8)</f>
-        <v>1733000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44235</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4">
+        <v>18729</v>
+      </c>
+      <c r="O8" s="4">
+        <f>SUM(N$7:N8)+M$6</f>
+        <v>372806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>44208</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>44228</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="5">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G9/I9</f>
+        <v>1500000</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -953,38 +1018,37 @@
         <v>18</v>
       </c>
       <c r="K9" s="1">
-        <v>44197</v>
-      </c>
-      <c r="L9" s="11">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12">
-        <f>SUM(L9:L$9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44242</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4">
+        <v>170000</v>
+      </c>
+      <c r="O9" s="4">
+        <f>SUM(N$7:N9)+M$6</f>
+        <v>542806</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>44209</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="6">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5">
         <v>0.94</v>
       </c>
       <c r="G10" s="4">
-        <v>7500000</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
-        <f>G10/I10</f>
-        <v>3750000</v>
+        <f t="shared" ref="H10" si="2">G10/I10</f>
+        <v>0</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -993,34 +1057,33 @@
         <v>18</v>
       </c>
       <c r="K10" s="1">
+        <v>44197</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <f>SUM(L10:L$10)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
         <v>44209</v>
       </c>
-      <c r="L10">
-        <v>200000</v>
-      </c>
-      <c r="M10" s="10">
-        <f>SUM(L$9:L10)</f>
-        <v>200000</v>
-      </c>
-      <c r="N10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.94099999999999995</v>
+      <c r="F11" s="6">
+        <v>0.94</v>
       </c>
       <c r="G11" s="4">
         <v>7500000</v>
@@ -1036,17 +1099,22 @@
         <v>18</v>
       </c>
       <c r="K11" s="1">
-        <v>44227</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="10">
-        <f>SUM(L$9:L11)</f>
+        <v>44209</v>
+      </c>
+      <c r="L11" s="4">
         <v>200000</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="4">
+        <f>SUM(L$10:L11)</f>
+        <v>200000</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1054,10 +1122,10 @@
         <v>44188</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="5">
         <v>0.94099999999999995</v>
@@ -1076,28 +1144,30 @@
         <v>18</v>
       </c>
       <c r="K12" s="1">
-        <v>44255</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="10">
-        <f>SUM(L$9:L12)</f>
+        <v>44227</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <f>SUM(L$10:L12)</f>
         <v>200000</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C13" s="2" t="s">
+        <v>44228</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
         <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
       </c>
       <c r="F13" s="5">
         <v>0.94099999999999995</v>
@@ -1116,28 +1186,32 @@
         <v>18</v>
       </c>
       <c r="K13" s="1">
-        <v>44286</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <f>SUM(L$9:L13)</f>
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44228</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
+        <v>300000</v>
+      </c>
+      <c r="O13" s="4">
+        <f>SUM(N$13:N13)+M$12</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>44188</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
       </c>
       <c r="F14" s="5">
         <v>0.94099999999999995</v>
@@ -1156,62 +1230,249 @@
         <v>18</v>
       </c>
       <c r="K14" s="1">
+        <v>44249</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4">
+        <v>400000</v>
+      </c>
+      <c r="O14" s="4">
+        <f>SUM(N$13:N14)+M$12</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44188</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="G15" s="4">
+        <v>7500000</v>
+      </c>
+      <c r="H15" s="4">
+        <f>G15/I15</f>
+        <v>3750000</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="1">
         <v>44316</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <f>SUM(L$9:L14)</f>
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44188</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="G16" s="4">
+        <v>7500000</v>
+      </c>
+      <c r="H16" s="4">
+        <f>G16/I16</f>
+        <v>3750000</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="1">
+        <v>44316</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
         <v>44173</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="F17" s="6">
         <v>0.9</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G17" s="4">
         <v>5300000</v>
       </c>
-      <c r="H15" s="4">
-        <f t="shared" ref="H15" si="2">G15/I15</f>
+      <c r="H17" s="4">
+        <f t="shared" ref="H17" si="3">G17/I17</f>
         <v>3533333.3333333335</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I17" s="7">
         <v>1.5</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="1">
+        <v>44197</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44173</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="1">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>5300000</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" ref="H18:H19" si="4">G18/I18</f>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="I18" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="1">
         <v>44227</v>
       </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44173</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>5300000</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="4"/>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="1">
+        <v>44227</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{E2470301-8F3C-4769-93D1-23C55ED5F843}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{C2A3FF95-20F0-42E1-A0B2-8408C11AE819}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
-    <hyperlink ref="C15" r:id="rId4" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
-    <hyperlink ref="C10" r:id="rId5" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
-    <hyperlink ref="C12" r:id="rId6" xr:uid="{73FB11BF-0AE6-49E9-83F1-5A1CEB8236AB}"/>
-    <hyperlink ref="C3" r:id="rId7" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{AE9291CE-08B0-4A7E-831F-624AB82E6F35}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
+    <hyperlink ref="C11" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
+    <hyperlink ref="C13" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
+    <hyperlink ref="C14" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId9"/>
   <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
@@ -1367,18 +1628,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1400,14 +1661,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1421,4 +1674,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
restored old file (backward compatibility, added new file with new structure
</commit_message>
<xml_diff>
--- a/data_vaccines.xlsx
+++ b/data_vaccines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DC0145-15ED-4B77-91A7-0142340774B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBAD2DD-E94C-4FD6-9C20-5ADDBFF3EED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
+    <workbookView xWindow="16752" yWindow="1356" windowWidth="12192" windowHeight="13320" xr2:uid="{903CCA78-31AC-4C43-8A11-60BB4F0FD4C5}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccine approval" sheetId="3" r:id="rId1"/>
@@ -35,12 +35,13 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={FE94EFC9-43E2-473A-8C67-92FC024C88A5}</author>
     <author>tc={10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}</author>
     <author>tc={DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}</author>
     <author>tc={21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}</author>
   </authors>
   <commentList>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{FE94EFC9-43E2-473A-8C67-92FC024C88A5}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -48,7 +49,7 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="I18" authorId="1" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+    <comment ref="I17" authorId="1" shapeId="0" xr:uid="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -56,7 +57,15 @@
     Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
       </text>
     </comment>
-    <comment ref="I19" authorId="2" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
+    <comment ref="I18" authorId="2" shapeId="0" xr:uid="{DEA883F4-A8BC-47C0-A45D-029EE9D3F93D}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</t>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="3" shapeId="0" xr:uid="{21DA53E9-4AC5-411F-AFA8-A01BFD6A8B13}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -69,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>country</t>
   </si>
@@ -155,26 +164,18 @@
     <t>https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert</t>
   </si>
   <si>
-    <t>shipping_volume_forecast</t>
-  </si>
-  <si>
-    <t>BAG pdf</t>
-  </si>
-  <si>
-    <t>https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/</t>
-  </si>
-  <si>
-    <t>shipping_volume_forecast_cummulated</t>
+    <t>https://www.cash.ch/news/politik/coronavirus-update-corona-bag-meldet-4020-neue-coronavirus-infektionen-schweiz-hat-233000-1688758</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -238,7 +239,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
@@ -251,10 +252,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -578,6 +581,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I15" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{FE94EFC9-43E2-473A-8C67-92FC024C88A5}">
+    <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
+  </threadedComment>
   <threadedComment ref="I17" dT="2021-01-11T14:32:58.02" personId="{4E5CC7C5-43C4-40CF-A9EA-62F40AE8BF26}" id="{10BF3F74-5FA4-4FDC-B3C2-C628B8C349E9}">
     <text>Quelle: https://www.srf.ch/news/schweiz/covid-impfung-in-der-schweiz-diese-impfstoffe-sind-noch-im-rennen-um-die-zulassung</text>
   </threadedComment>
@@ -594,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828B207B-0EB6-4EF4-88FB-421592296A82}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -644,21 +650,17 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -695,18 +697,17 @@
       <c r="K2" s="1">
         <v>44184</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2">
         <f>SUM(L$2:L2)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
       <c r="O2" s="4"/>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -743,18 +744,17 @@
       <c r="K3" s="1">
         <v>44185</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <v>107000</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3">
         <f>SUM(L$2:L3)</f>
         <v>107000</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
       <c r="O3" s="4"/>
-      <c r="P3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -791,28 +791,27 @@
       <c r="K4" s="1">
         <v>44200</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <v>126000</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <f>SUM(L$2:L4)</f>
         <v>233000</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
       <c r="O4" s="4"/>
-      <c r="P4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>44228</v>
+        <v>44201</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -827,7 +826,7 @@
         <v>3000000</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5" si="0">G5/I5</f>
+        <f t="shared" ref="H5:H9" si="0">G5/I5</f>
         <v>1500000</v>
       </c>
       <c r="I5" s="4">
@@ -837,16 +836,18 @@
         <v>18</v>
       </c>
       <c r="K5" s="1">
-        <v>44220</v>
-      </c>
-      <c r="L5" s="4">
-        <f>M5-M4</f>
-        <v>38400</v>
-      </c>
-      <c r="M5" s="4">
-        <v>271400</v>
-      </c>
-      <c r="N5" s="4"/>
+        <v>44227</v>
+      </c>
+      <c r="L5">
+        <v>500000</v>
+      </c>
+      <c r="M5">
+        <f>SUM(L$2:L5)</f>
+        <v>733000</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -854,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="1">
-        <v>44228</v>
+        <v>44201</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -872,7 +873,7 @@
         <v>3000000</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" ref="H6" si="1">G6/I6</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="I6" s="4">
@@ -882,16 +883,15 @@
         <v>18</v>
       </c>
       <c r="K6" s="1">
-        <v>44223</v>
-      </c>
-      <c r="L6" s="4">
-        <f>M6-M5</f>
-        <v>60460</v>
-      </c>
-      <c r="M6" s="4">
-        <v>331860</v>
-      </c>
-      <c r="N6" s="4"/>
+        <v>44255</v>
+      </c>
+      <c r="L6">
+        <v>500000</v>
+      </c>
+      <c r="M6">
+        <f>SUM(L$2:L6)</f>
+        <v>1233000</v>
+      </c>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -899,10 +899,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>44228</v>
+        <v>44201</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -917,7 +917,7 @@
         <v>3000000</v>
       </c>
       <c r="H7" s="4">
-        <f>G7/I7</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="I7" s="4">
@@ -927,29 +927,26 @@
         <v>18</v>
       </c>
       <c r="K7" s="1">
-        <v>44228</v>
-      </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4">
-        <v>22217</v>
-      </c>
-      <c r="O7" s="4">
-        <f>SUM(N$7:N7)+M$6</f>
-        <v>354077</v>
-      </c>
-      <c r="P7" t="s">
-        <v>21</v>
-      </c>
+        <v>44286</v>
+      </c>
+      <c r="L7">
+        <v>500000</v>
+      </c>
+      <c r="M7">
+        <f>SUM(L$2:L7)</f>
+        <v>1733000</v>
+      </c>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1">
-        <v>44228</v>
+        <v>44201</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -964,7 +961,7 @@
         <v>3000000</v>
       </c>
       <c r="H8" s="4">
-        <f>G8/I8</f>
+        <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
       <c r="I8" s="4">
@@ -974,42 +971,37 @@
         <v>18</v>
       </c>
       <c r="K8" s="1">
-        <v>44235</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4">
-        <v>18729</v>
-      </c>
-      <c r="O8" s="4">
-        <f>SUM(N$7:N8)+M$6</f>
-        <v>372806</v>
-      </c>
+        <v>44316</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>SUM(L$2:L8)</f>
+        <v>1733000</v>
+      </c>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>44228</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>44208</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F9" s="5">
-        <v>0.9</v>
+        <v>0.94</v>
       </c>
       <c r="G9" s="4">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4">
-        <f>G9/I9</f>
-        <v>1500000</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -1018,37 +1010,39 @@
         <v>18</v>
       </c>
       <c r="K9" s="1">
-        <v>44242</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4">
-        <v>170000</v>
-      </c>
-      <c r="O9" s="4">
-        <f>SUM(N$7:N9)+M$6</f>
-        <v>542806</v>
-      </c>
+        <v>44197</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <f>SUM(L9:L$9)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>44208</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>44209</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>0.94</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>7500000</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" ref="H10" si="2">G10/I10</f>
-        <v>0</v>
+        <f>G10/I10</f>
+        <v>3750000</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -1057,16 +1051,18 @@
         <v>18</v>
       </c>
       <c r="K10" s="1">
-        <v>44197</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <f>SUM(L10:L$10)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="4"/>
+        <v>44209</v>
+      </c>
+      <c r="L10">
+        <v>200000</v>
+      </c>
+      <c r="M10" s="13">
+        <f>SUM(L$9:L10)</f>
+        <v>200000</v>
+      </c>
+      <c r="N10" t="s">
+        <v>19</v>
+      </c>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1074,16 +1070,16 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>44209</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>27</v>
+        <v>44188</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="6">
-        <v>0.94</v>
+      <c r="F11" s="5">
+        <v>0.94099999999999995</v>
       </c>
       <c r="G11" s="4">
         <v>7500000</v>
@@ -1099,20 +1095,16 @@
         <v>18</v>
       </c>
       <c r="K11" s="1">
-        <v>44209</v>
-      </c>
-      <c r="L11" s="4">
+        <v>44227</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <f>SUM(L$9:L11)</f>
         <v>200000</v>
       </c>
-      <c r="M11" s="4">
-        <f>SUM(L$10:L11)</f>
-        <v>200000</v>
-      </c>
-      <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1144,16 +1136,15 @@
         <v>18</v>
       </c>
       <c r="K12" s="1">
-        <v>44227</v>
-      </c>
-      <c r="L12" s="4">
+        <v>44255</v>
+      </c>
+      <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="4">
-        <f>SUM(L$10:L12)</f>
+      <c r="M12" s="13">
+        <f>SUM(L$9:L12)</f>
         <v>200000</v>
       </c>
-      <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1161,10 +1152,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>44228</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>44188</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -1186,19 +1177,16 @@
         <v>18</v>
       </c>
       <c r="K13" s="1">
-        <v>44228</v>
-      </c>
-      <c r="L13" s="4">
+        <v>44286</v>
+      </c>
+      <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4">
-        <v>300000</v>
-      </c>
-      <c r="O13" s="4">
-        <f>SUM(N$13:N13)+M$12</f>
-        <v>500000</v>
-      </c>
+      <c r="M13" s="13">
+        <f>SUM(L$9:L13)</f>
+        <v>200000</v>
+      </c>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1207,8 +1195,8 @@
       <c r="B14" s="1">
         <v>44188</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>30</v>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -1230,246 +1218,110 @@
         <v>18</v>
       </c>
       <c r="K14" s="1">
-        <v>44249</v>
-      </c>
-      <c r="L14" s="4">
+        <v>44316</v>
+      </c>
+      <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4">
-        <v>400000</v>
-      </c>
-      <c r="O14" s="4">
-        <f>SUM(N$13:N14)+M$12</f>
-        <v>900000</v>
-      </c>
+      <c r="M14" s="13">
+        <f>SUM(L$9:L14)</f>
+        <v>200000</v>
+      </c>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>44173</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.94099999999999995</v>
+        <v>26</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.9</v>
       </c>
       <c r="G15" s="4">
-        <v>7500000</v>
+        <v>5300000</v>
       </c>
       <c r="H15" s="4">
-        <f>G15/I15</f>
-        <v>3750000</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2</v>
+        <f t="shared" ref="H15" si="1">G15/I15</f>
+        <v>3533333.3333333335</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.5</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="K15" s="1">
-        <v>44316</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+        <v>44227</v>
+      </c>
+      <c r="L15"/>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44188</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="G16" s="4">
-        <v>7500000</v>
-      </c>
-      <c r="H16" s="4">
-        <f>G16/I16</f>
-        <v>3750000</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="1">
-        <v>44316</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="K16" s="1"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="G17" s="4">
-        <v>5300000</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" ref="H17" si="3">G17/I17</f>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="I17" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="J17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="1">
-        <v>44197</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="G18" s="4">
-        <v>5300000</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" ref="H18:H19" si="4">G18/I18</f>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="I18" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="J18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="1">
-        <v>44227</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0</v>
-      </c>
-      <c r="O18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44173</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="G19" s="4">
-        <v>5300000</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="4"/>
-        <v>3533333.3333333335</v>
-      </c>
-      <c r="I19" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="J19" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="1">
-        <v>44227</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C26" s="11"/>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="8"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="7"/>
+      <c r="K17" s="1"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="8"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="7"/>
+      <c r="K18" s="1"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="8"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="7"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C26" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E8567AFD-F948-4690-A799-1E8401B37C92}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{CCDB50F2-345E-4CFB-BAA2-0C0D2ABAD8F6}"/>
-    <hyperlink ref="C11" r:id="rId3" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{E80E64FB-39B3-4B99-9F5B-AC7265D157AD}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{246D7B2B-C6AC-4855-A710-0B7EB86FC31B}"/>
-    <hyperlink ref="C13" r:id="rId5" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{65B1E0B5-520F-417B-A93C-D2870E54C409}"/>
-    <hyperlink ref="C18" r:id="rId6" xr:uid="{8099B6F1-170E-4CA9-894B-6A11EACA7DE3}"/>
-    <hyperlink ref="C19" r:id="rId7" xr:uid="{B7E311B5-9C0F-43D4-B281-2686EEC34209}"/>
-    <hyperlink ref="C14" r:id="rId8" tooltip="https://interaktiv.tagesanzeiger.ch/2020/wo-die-schweiz-im-grossen-impfrennen-steht/" xr:uid="{1A41E538-3658-4ECB-A121-4CB5B41913A5}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{A30FBD76-A843-4D0E-875D-7C6E2A8DC3A7}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{BF68BDCF-FA52-45A0-9D52-2DC8853728E4}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{6410A865-6E4B-4CB9-A30D-8946B3CA82B1}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{977D1EF0-053E-4B70-AC02-5BE60265B6B7}"/>
+    <hyperlink ref="C10" r:id="rId5" tooltip="https://www.srf.ch/news/wirtschaft/die-logistik-hinter-moderna-wie-die-schweiz-die-versorgung-mit-dem-neuen-impfstoff-sichert" xr:uid="{5AFC4ADB-A3E7-4966-9275-15AC19128A4F}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{BD211785-E33E-4A26-AA23-D7BDFDD30FF4}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{8CDB2F45-0D61-413A-8159-5B93393F9FF7}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{7CB87138-D10B-4F21-98AD-BB490221A307}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="360" r:id="rId9"/>
@@ -1478,6 +1330,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100DED90A92496A7744ABCE13896B9F92DA" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b49787f72d67ac0aa2c3a374ebf068f2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d5bda608be47ebbf9612181af6292e1" ns2:_="">
     <xsd:import namespace="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
@@ -1627,12 +1485,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1643,6 +1495,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9893CF25-92F4-48D2-9BBB-695FEE2AB90C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1660,22 +1528,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2D919F7-6F5F-4E1C-ABD8-8F275E6A7768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cb223a9f-5a50-4cf6-bd48-e7fe6a835b02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C96820-C391-4B7C-A57F-E7A178B5A878}">
   <ds:schemaRefs>

</xml_diff>